<commit_message>
Fixed ED UK grade missing
</commit_message>
<xml_diff>
--- a/data/ED/program_url_pair.xlsx
+++ b/data/ED/program_url_pair.xlsx
@@ -1938,7 +1938,7 @@
       <c r="A84" t="inlineStr">
         <is>
           <t>data and artificial intelligence ethics  
-    subject to approval</t>
+    msc, pgdip, pgcert</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1957,7 +1957,7 @@
         <is>
           <t>online
     data and artificial intelligence ethics (online learning)   
-    subject to approval</t>
+    msc, pgdip, pgcert</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">

</xml_diff>